<commit_message>
updated task and context
</commit_message>
<xml_diff>
--- a/forms/app/test.xlsx
+++ b/forms/app/test.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="75">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -154,6 +154,15 @@
     <t xml:space="preserve">end group</t>
   </si>
   <si>
+    <t xml:space="preserve">calculate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">patient_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../inputs/contact/name</t>
+  </si>
+  <si>
     <t xml:space="preserve">begin_group</t>
   </si>
   <si>
@@ -166,22 +175,72 @@
     <t xml:space="preserve">Description of maternity services</t>
   </si>
   <si>
-    <t xml:space="preserve">note</t>
-  </si>
-  <si>
-    <t xml:space="preserve">……… जाँच</t>
-  </si>
-  <si>
-    <t xml:space="preserve">....... Service </t>
-  </si>
-  <si>
     <t xml:space="preserve">select_one one</t>
   </si>
   <si>
     <t xml:space="preserve">ch_1</t>
   </si>
   <si>
-    <t xml:space="preserve">please choose </t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">कृपया ${</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">patient_name}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> को अवस्था चयन गर्नुहोस् I</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Please select the condition of ${</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">patient_name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">}</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">end_group</t>
@@ -196,25 +255,37 @@
     <t xml:space="preserve">c_1</t>
   </si>
   <si>
-    <t xml:space="preserve">choice 1 </t>
+    <t xml:space="preserve">चिन्ता</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anxiety</t>
   </si>
   <si>
     <t xml:space="preserve">c_2</t>
   </si>
   <si>
-    <t xml:space="preserve">choice 2 </t>
+    <t xml:space="preserve">उदासीपन</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depression</t>
   </si>
   <si>
     <t xml:space="preserve">c_3</t>
   </si>
   <si>
-    <t xml:space="preserve">choice 3 </t>
+    <t xml:space="preserve">मधुमेह</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diabetes</t>
   </si>
   <si>
     <t xml:space="preserve">c_4</t>
   </si>
   <si>
-    <t xml:space="preserve">Choice 4</t>
+    <t xml:space="preserve">उच्च रक्तचाप</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hypertension</t>
   </si>
   <si>
     <t xml:space="preserve">form_title</t>
@@ -260,7 +331,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -321,6 +392,18 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="8"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF00FF00"/>
       <name val="Arial"/>
@@ -328,7 +411,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -344,19 +427,37 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE2E2E2"/>
-        <bgColor rgb="FFD9EAD3"/>
+        <bgColor rgb="FFDDE8CB"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9EAD3"/>
-        <bgColor rgb="FFE2E2E2"/>
+        <bgColor rgb="FFDDE8CB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAFD095"/>
+        <bgColor rgb="FF93C47D"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDE8CB"/>
+        <bgColor rgb="FFD9EAD3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D2E9"/>
         <bgColor rgb="FFCFCFCF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF93C47D"/>
+        <bgColor rgb="FFAFD095"/>
       </patternFill>
     </fill>
     <fill>
@@ -368,7 +469,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA2C4C9"/>
-        <bgColor rgb="FFB4A7D6"/>
+        <bgColor rgb="FFAFD095"/>
       </patternFill>
     </fill>
     <fill>
@@ -433,7 +534,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -470,7 +571,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -478,7 +591,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -486,15 +603,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -504,6 +621,10 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -539,7 +660,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFDDE8CB"/>
       <rgbColor rgb="FFE2E2E2"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -563,12 +684,12 @@
       <rgbColor rgb="FFE6B8AF"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFAFD095"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF93C47D"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -592,10 +713,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H28" activeCellId="0" sqref="H28"/>
+      <selection pane="bottomLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -912,11 +1033,32 @@
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
+    <row r="13" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="L13" s="10"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8"/>
@@ -925,57 +1067,51 @@
       <c r="D14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="9" t="s">
+      <c r="A15" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="B15" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="13" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+    </row>
+    <row r="17" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8"/>
@@ -1000,20 +1136,20 @@
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8"/>
@@ -1026,7 +1162,7 @@
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
-      <c r="F25" s="12"/>
+      <c r="F25" s="16"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="8"/>
@@ -1035,119 +1171,119 @@
       <c r="D26" s="8"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
+      <c r="A28" s="17"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
+      <c r="A29" s="17"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="13"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
+      <c r="A31" s="17"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
+      <c r="A32" s="17"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="13"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
+      <c r="A33" s="17"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="13"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
+      <c r="A34" s="17"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="13"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
+      <c r="A35" s="17"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
+      <c r="A36" s="17"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="13"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
+      <c r="A37" s="17"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="13"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
+      <c r="A38" s="17"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="13"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="F39" s="12"/>
+      <c r="A39" s="17"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="F39" s="16"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="13"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
+      <c r="A40" s="17"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="14"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
+      <c r="A42" s="18"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="14"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
+      <c r="A43" s="18"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="14"/>
-      <c r="B44" s="14"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
+      <c r="A44" s="18"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="15"/>
-      <c r="B46" s="15"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="15"/>
+      <c r="A46" s="19"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="15"/>
-      <c r="B47" s="15"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
+      <c r="A47" s="19"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="15"/>
-      <c r="B48" s="15"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
+      <c r="A48" s="19"/>
+      <c r="B48" s="19"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="19"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1168,22 +1304,22 @@
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="17" t="s">
+      <c r="A1" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="21" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="3"/>
@@ -1209,60 +1345,60 @@
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="B3" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>55</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>58</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>57</v>
+      <c r="A5" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>61</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1292,29 +1428,29 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1" s="18" t="s">
+      <c r="A1" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="B1" s="23" t="s">
         <v>64</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>69</v>
       </c>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -1338,22 +1474,22 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C2" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>